<commit_message>
before elimination of J7
</commit_message>
<xml_diff>
--- a/OTA補償回路定数計算.xlsx
+++ b/OTA補償回路定数計算.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yudun\Documents\KiCad\8.0\projects\chibarobo_board_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E486B0C-6EE5-4134-8DD7-C6DEDB92747D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226D7DEC-35AE-4F8B-8BE8-480F87CA51DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{57ABD89D-B5C3-471B-A426-04A42F11EAD5}"/>
   </bookViews>
@@ -95,7 +95,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="0.0000000000E+00"/>
+    <numFmt numFmtId="176" formatCode="0.0000000000E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -171,10 +171,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -514,7 +514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5E6815-465E-45EB-BC9C-9E7C5372E074}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -577,38 +577,38 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
-        <v>590000</v>
+        <v>59000</v>
       </c>
       <c r="B2" s="1">
-        <v>3.3E-10</v>
+        <v>3.3000000000000002E-9</v>
       </c>
       <c r="C2" s="2">
         <f>1/(2*PI()*A2*B2)</f>
-        <v>817.43679040521488</v>
+        <v>817.43679040521477</v>
       </c>
       <c r="D2" s="1">
-        <v>1.8E-12</v>
+        <v>1.7999999999999999E-11</v>
       </c>
       <c r="E2" s="2">
         <f>1/(2*PI()*A2*D2)</f>
         <v>149863.41157428941</v>
       </c>
       <c r="F2" s="1">
-        <v>8.1999999999999996E-10</v>
+        <v>8.2000000000000006E-9</v>
       </c>
       <c r="G2" s="2">
         <f>(12*A2*F2)/(2*PI()*0.0001*1.5*0.00022)</f>
-        <v>27999.695079221437</v>
+        <v>27999.695079221445</v>
       </c>
       <c r="H2" s="1">
-        <v>3480</v>
+        <v>348</v>
       </c>
       <c r="I2" s="2">
         <f>1/(2*PI()*F2*H2)</f>
-        <v>55773.389084628318</v>
+        <v>55773.389084628303</v>
       </c>
       <c r="J2" s="1">
-        <v>177000</v>
+        <v>17700</v>
       </c>
       <c r="K2" s="2">
         <f>1/(2*PI()*F2*(J2+H2))</f>
@@ -616,11 +616,11 @@
       </c>
       <c r="L2" s="2">
         <f>0.6/(7.5-0.6)*J2</f>
-        <v>15391.304347826086</v>
+        <v>1539.1304347826087</v>
       </c>
       <c r="M2" s="2">
         <f>(J2*L2*H2)/(J2*H2+L2*H2+J2*L2)</f>
-        <v>2793.4693877551017</v>
+        <v>279.34693877551024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>